<commit_message>
Add all validations checks to validate.py
</commit_message>
<xml_diff>
--- a/tests/Delivered.xlsx
+++ b/tests/Delivered.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" state="visible" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Key</t>
   </si>
@@ -88,6 +88,9 @@
     <t>dfdsf</t>
   </si>
   <si>
+    <t>dfdsfe</t>
+  </si>
+  <si>
     <t>dfsfd</t>
   </si>
   <si>
@@ -109,7 +112,10 @@
     <t>dsf</t>
   </si>
   <si>
-    <t>sdffds</t>
+    <t>sdffdsd</t>
+  </si>
+  <si>
+    <t>sdffdse</t>
   </si>
   <si>
     <t>weer</t>
@@ -1345,7 +1351,7 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7">
@@ -1353,7 +1359,7 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1389,7 +1395,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3">
@@ -1397,7 +1403,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4">
@@ -1405,7 +1411,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5">
@@ -1421,7 +1427,7 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7">
@@ -1429,7 +1435,7 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1465,7 +1471,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3">
@@ -1473,7 +1479,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4">
@@ -1481,7 +1487,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5">
@@ -1489,7 +1495,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6">
@@ -1497,7 +1503,7 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7">
@@ -1505,7 +1511,7 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>